<commit_message>
Updated control board schematics and board layout
</commit_message>
<xml_diff>
--- a/Schematics/Control Board/BOM.xlsx
+++ b/Schematics/Control Board/BOM.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryann\OneDrive\Documents\GitHub\FRC-4901-Garnet-Squadron\Schematics\Control Board\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="9465"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="22980" windowHeight="9465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
   <si>
     <t>Qty</t>
   </si>
@@ -373,12 +378,24 @@
   </si>
   <si>
     <t>311-1358-6-ND</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Voltage Drop</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Voltage Supply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000"/>
@@ -431,7 +448,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -457,6 +474,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -467,6 +486,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -515,7 +537,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,7 +572,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,12 +2093,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1.85</v>
+      </c>
+      <c r="D2" s="12">
+        <f>(B2-C2)/$B$7</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="12">
+        <f t="shared" ref="D3:D5" si="0">(B3-C3)/$B$7</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="12">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>170.00000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>